<commit_message>
get no longer creates duplicate files
</commit_message>
<xml_diff>
--- a/Output/QC.xlsx
+++ b/Output/QC.xlsx
@@ -34,7 +34,7 @@
     <t>New Efficiency</t>
   </si>
   <si>
-    <t>C:\Users\paul.jones\Documents\GitHub\ModiffyEfficiency\ModiffyEfficiency\Output\Output Files\Characterization 011020-950.xlsx</t>
+    <t>C:/Users/paul.jones/Documents/GitHub/ModiffyEfficiency/ModiffyEfficiency/surveys\Characterization 011020-950.xlsx</t>
   </si>
   <si>
     <t>&lt;Worksheet "Survey Sheet (2)"&gt;</t>
@@ -46,7 +46,7 @@
     <t>&lt;Worksheet "2360-190602"&gt;</t>
   </si>
   <si>
-    <t>C:\Users\paul.jones\Documents\GitHub\ModiffyEfficiency\ModiffyEfficiency\Output\Output Files\Characterization 012320-1045.xlsx</t>
+    <t>C:/Users/paul.jones/Documents/GitHub/ModiffyEfficiency/ModiffyEfficiency/surveys\Characterization 012320-1045.xlsx</t>
   </si>
   <si>
     <t>&lt;Worksheet "Scan and Data"&gt;</t>
@@ -55,49 +55,49 @@
     <t>268475/PR289416</t>
   </si>
   <si>
-    <t>C:\Users\paul.jones\Documents\GitHub\ModiffyEfficiency\ModiffyEfficiency\Output\Output Files\Characterization 081919-196.xlsx</t>
+    <t>C:/Users/paul.jones/Documents/GitHub/ModiffyEfficiency/ModiffyEfficiency/surveys\Characterization 081919-196.xlsx</t>
   </si>
   <si>
     <t>170550/PR312880</t>
   </si>
   <si>
-    <t>C:\Users\paul.jones\Documents\GitHub\ModiffyEfficiency\ModiffyEfficiency\Output\Output Files\Characterization 082019-198.xlsx</t>
-  </si>
-  <si>
-    <t>C:\Users\paul.jones\Documents\GitHub\ModiffyEfficiency\ModiffyEfficiency\Output\Output Files\Characterization 102819-524.xlsx</t>
+    <t>C:/Users/paul.jones/Documents/GitHub/ModiffyEfficiency/ModiffyEfficiency/surveys\Characterization 082019-198.xlsx</t>
+  </si>
+  <si>
+    <t>C:/Users/paul.jones/Documents/GitHub/ModiffyEfficiency/ModiffyEfficiency/surveys\Characterization 102819-524.xlsx</t>
   </si>
   <si>
     <t>227413/PR295918</t>
   </si>
   <si>
-    <t>C:\Users\paul.jones\Documents\GitHub\ModiffyEfficiency\ModiffyEfficiency\Output\Output Files\Characterization 103019-545.xlsx</t>
+    <t>C:/Users/paul.jones/Documents/GitHub/ModiffyEfficiency/ModiffyEfficiency/surveys\Characterization 103019-545.xlsx</t>
   </si>
   <si>
     <t>170573/PR295917</t>
   </si>
   <si>
-    <t>C:\Users\paul.jones\Documents\GitHub\ModiffyEfficiency\ModiffyEfficiency\Output\Output Files\Characterization 110119-562.xlsx</t>
+    <t>C:/Users/paul.jones/Documents/GitHub/ModiffyEfficiency/ModiffyEfficiency/surveys\Characterization 110119-562.xlsx</t>
   </si>
   <si>
     <t>234860/PR289402</t>
   </si>
   <si>
-    <t>C:\Users\paul.jones\Documents\GitHub\ModiffyEfficiency\ModiffyEfficiency\Output\Output Files\Characterization 110819-620.xlsx</t>
+    <t>C:/Users/paul.jones/Documents/GitHub/ModiffyEfficiency/ModiffyEfficiency/surveys\Characterization 110819-620.xlsx</t>
   </si>
   <si>
     <t>227431/PR289429</t>
   </si>
   <si>
-    <t>C:\Users\paul.jones\Documents\GitHub\ModiffyEfficiency\ModiffyEfficiency\Output\Output Files\Characterization 110919-635.xlsx</t>
+    <t>C:/Users/paul.jones/Documents/GitHub/ModiffyEfficiency/ModiffyEfficiency/surveys\Characterization 110919-635.xlsx</t>
   </si>
   <si>
     <t>&lt;Worksheet "2360-190602 "&gt;</t>
   </si>
   <si>
-    <t>C:\Users\paul.jones\Documents\GitHub\ModiffyEfficiency\ModiffyEfficiency\Output\Output Files\Characterization 110919-636.xlsx</t>
-  </si>
-  <si>
-    <t>C:\Users\paul.jones\Documents\GitHub\ModiffyEfficiency\ModiffyEfficiency\Output\Output Files\INIS-012020-1020.xlsx</t>
+    <t>C:/Users/paul.jones/Documents/GitHub/ModiffyEfficiency/ModiffyEfficiency/surveys\Characterization 110919-636.xlsx</t>
+  </si>
+  <si>
+    <t>C:/Users/paul.jones/Documents/GitHub/ModiffyEfficiency/ModiffyEfficiency/surveys\INIS-012020-1020.xlsx</t>
   </si>
   <si>
     <t>&lt;Worksheet "Survey"&gt;</t>
@@ -106,7 +106,7 @@
     <t>251035/PR293951</t>
   </si>
   <si>
-    <t>C:\Users\paul.jones\Documents\GitHub\ModiffyEfficiency\ModiffyEfficiency\Output\Output Files\INIS-061620-1794.xlsx</t>
+    <t>C:/Users/paul.jones/Documents/GitHub/ModiffyEfficiency/ModiffyEfficiency/surveys\INIS-061620-1794.xlsx</t>
   </si>
   <si>
     <t>227404/PR389087</t>
@@ -115,13 +115,13 @@
     <t>&lt;Worksheet "Scan and Data (2)"&gt;</t>
   </si>
   <si>
-    <t>C:\Users\paul.jones\Documents\GitHub\ModiffyEfficiency\ModiffyEfficiency\Output\Output Files\INIS-070920-1966.xlsx</t>
+    <t>C:/Users/paul.jones/Documents/GitHub/ModiffyEfficiency/ModiffyEfficiency/surveys\INIS-070920-1966.xlsx</t>
   </si>
   <si>
     <t>268409/PR295781</t>
   </si>
   <si>
-    <t>C:\Users\paul.jones\Documents\GitHub\ModiffyEfficiency\ModiffyEfficiency\Output\Output Files\INIS-071020-1968.xlsx</t>
+    <t>C:/Users/paul.jones/Documents/GitHub/ModiffyEfficiency/ModiffyEfficiency/surveys\INIS-071020-1968.xlsx</t>
   </si>
   <si>
     <t>&lt;Worksheet "Sub-Basement"&gt;</t>
@@ -160,7 +160,7 @@
     <t>&lt;Worksheet "9th Floor"&gt;</t>
   </si>
   <si>
-    <t>C:\Users\paul.jones\Documents\GitHub\ModiffyEfficiency\ModiffyEfficiency\Output\Output Files\INIS-FSS-010820-001 - Rev 4.xlsx</t>
+    <t>C:/Users/paul.jones/Documents/GitHub/ModiffyEfficiency/ModiffyEfficiency/surveys\INIS-FSS-010820-001 - Rev 4.xlsx</t>
   </si>
   <si>
     <t>&lt;Worksheet "FSS-001"&gt;</t>
@@ -286,7 +286,7 @@
     <t>227401/PR312929</t>
   </si>
   <si>
-    <t>C:\Users\paul.jones\Documents\GitHub\ModiffyEfficiency\ModiffyEfficiency\Output\Output Files\INIS-FSS-052820-006 (HRT 11-13).xlsx</t>
+    <t>C:/Users/paul.jones/Documents/GitHub/ModiffyEfficiency/ModiffyEfficiency/surveys\INIS-FSS-052820-006 (HRT 11-13).xlsx</t>
   </si>
   <si>
     <t>&lt;Worksheet "Systematic SDS"&gt;</t>

</xml_diff>

<commit_message>
Fixed not displaying correct old efficiency
</commit_message>
<xml_diff>
--- a/Output/QC.xlsx
+++ b/Output/QC.xlsx
@@ -34,7 +34,7 @@
     <t>New Efficiency</t>
   </si>
   <si>
-    <t>C:/Users/paul.jones/Documents/GitHub/ModiffyEfficiency/ModiffyEfficiency/surveys\Characterization 011020-950.xlsx</t>
+    <t>C:\Users\paul.jones\Documents\GitHub\ModiffyEfficiency\ModiffyEfficiency\Output\Output Files\Characterization 011020-950.xlsx</t>
   </si>
   <si>
     <t>&lt;Worksheet "Survey Sheet (2)"&gt;</t>
@@ -46,7 +46,7 @@
     <t>&lt;Worksheet "2360-190602"&gt;</t>
   </si>
   <si>
-    <t>C:/Users/paul.jones/Documents/GitHub/ModiffyEfficiency/ModiffyEfficiency/surveys\Characterization 012320-1045.xlsx</t>
+    <t>C:\Users\paul.jones\Documents\GitHub\ModiffyEfficiency\ModiffyEfficiency\Output\Output Files\Characterization 012320-1045.xlsx</t>
   </si>
   <si>
     <t>&lt;Worksheet "Scan and Data"&gt;</t>
@@ -55,49 +55,49 @@
     <t>268475/PR289416</t>
   </si>
   <si>
-    <t>C:/Users/paul.jones/Documents/GitHub/ModiffyEfficiency/ModiffyEfficiency/surveys\Characterization 081919-196.xlsx</t>
+    <t>C:\Users\paul.jones\Documents\GitHub\ModiffyEfficiency\ModiffyEfficiency\Output\Output Files\Characterization 081919-196.xlsx</t>
   </si>
   <si>
     <t>170550/PR312880</t>
   </si>
   <si>
-    <t>C:/Users/paul.jones/Documents/GitHub/ModiffyEfficiency/ModiffyEfficiency/surveys\Characterization 082019-198.xlsx</t>
-  </si>
-  <si>
-    <t>C:/Users/paul.jones/Documents/GitHub/ModiffyEfficiency/ModiffyEfficiency/surveys\Characterization 102819-524.xlsx</t>
+    <t>C:\Users\paul.jones\Documents\GitHub\ModiffyEfficiency\ModiffyEfficiency\Output\Output Files\Characterization 082019-198.xlsx</t>
+  </si>
+  <si>
+    <t>C:\Users\paul.jones\Documents\GitHub\ModiffyEfficiency\ModiffyEfficiency\Output\Output Files\Characterization 102819-524.xlsx</t>
   </si>
   <si>
     <t>227413/PR295918</t>
   </si>
   <si>
-    <t>C:/Users/paul.jones/Documents/GitHub/ModiffyEfficiency/ModiffyEfficiency/surveys\Characterization 103019-545.xlsx</t>
+    <t>C:\Users\paul.jones\Documents\GitHub\ModiffyEfficiency\ModiffyEfficiency\Output\Output Files\Characterization 103019-545.xlsx</t>
   </si>
   <si>
     <t>170573/PR295917</t>
   </si>
   <si>
-    <t>C:/Users/paul.jones/Documents/GitHub/ModiffyEfficiency/ModiffyEfficiency/surveys\Characterization 110119-562.xlsx</t>
+    <t>C:\Users\paul.jones\Documents\GitHub\ModiffyEfficiency\ModiffyEfficiency\Output\Output Files\Characterization 110119-562.xlsx</t>
   </si>
   <si>
     <t>234860/PR289402</t>
   </si>
   <si>
-    <t>C:/Users/paul.jones/Documents/GitHub/ModiffyEfficiency/ModiffyEfficiency/surveys\Characterization 110819-620.xlsx</t>
+    <t>C:\Users\paul.jones\Documents\GitHub\ModiffyEfficiency\ModiffyEfficiency\Output\Output Files\Characterization 110819-620.xlsx</t>
   </si>
   <si>
     <t>227431/PR289429</t>
   </si>
   <si>
-    <t>C:/Users/paul.jones/Documents/GitHub/ModiffyEfficiency/ModiffyEfficiency/surveys\Characterization 110919-635.xlsx</t>
+    <t>C:\Users\paul.jones\Documents\GitHub\ModiffyEfficiency\ModiffyEfficiency\Output\Output Files\Characterization 110919-635.xlsx</t>
   </si>
   <si>
     <t>&lt;Worksheet "2360-190602 "&gt;</t>
   </si>
   <si>
-    <t>C:/Users/paul.jones/Documents/GitHub/ModiffyEfficiency/ModiffyEfficiency/surveys\Characterization 110919-636.xlsx</t>
-  </si>
-  <si>
-    <t>C:/Users/paul.jones/Documents/GitHub/ModiffyEfficiency/ModiffyEfficiency/surveys\INIS-012020-1020.xlsx</t>
+    <t>C:\Users\paul.jones\Documents\GitHub\ModiffyEfficiency\ModiffyEfficiency\Output\Output Files\Characterization 110919-636.xlsx</t>
+  </si>
+  <si>
+    <t>C:\Users\paul.jones\Documents\GitHub\ModiffyEfficiency\ModiffyEfficiency\Output\Output Files\INIS-012020-1020.xlsx</t>
   </si>
   <si>
     <t>&lt;Worksheet "Survey"&gt;</t>
@@ -106,7 +106,7 @@
     <t>251035/PR293951</t>
   </si>
   <si>
-    <t>C:/Users/paul.jones/Documents/GitHub/ModiffyEfficiency/ModiffyEfficiency/surveys\INIS-061620-1794.xlsx</t>
+    <t>C:\Users\paul.jones\Documents\GitHub\ModiffyEfficiency\ModiffyEfficiency\Output\Output Files\INIS-061620-1794.xlsx</t>
   </si>
   <si>
     <t>227404/PR389087</t>
@@ -115,13 +115,13 @@
     <t>&lt;Worksheet "Scan and Data (2)"&gt;</t>
   </si>
   <si>
-    <t>C:/Users/paul.jones/Documents/GitHub/ModiffyEfficiency/ModiffyEfficiency/surveys\INIS-070920-1966.xlsx</t>
+    <t>C:\Users\paul.jones\Documents\GitHub\ModiffyEfficiency\ModiffyEfficiency\Output\Output Files\INIS-070920-1966.xlsx</t>
   </si>
   <si>
     <t>268409/PR295781</t>
   </si>
   <si>
-    <t>C:/Users/paul.jones/Documents/GitHub/ModiffyEfficiency/ModiffyEfficiency/surveys\INIS-071020-1968.xlsx</t>
+    <t>C:\Users\paul.jones\Documents\GitHub\ModiffyEfficiency\ModiffyEfficiency\Output\Output Files\INIS-071020-1968.xlsx</t>
   </si>
   <si>
     <t>&lt;Worksheet "Sub-Basement"&gt;</t>
@@ -160,7 +160,7 @@
     <t>&lt;Worksheet "9th Floor"&gt;</t>
   </si>
   <si>
-    <t>C:/Users/paul.jones/Documents/GitHub/ModiffyEfficiency/ModiffyEfficiency/surveys\INIS-FSS-010820-001 - Rev 4.xlsx</t>
+    <t>C:\Users\paul.jones\Documents\GitHub\ModiffyEfficiency\ModiffyEfficiency\Output\Output Files\INIS-FSS-010820-001 - Rev 4.xlsx</t>
   </si>
   <si>
     <t>&lt;Worksheet "FSS-001"&gt;</t>
@@ -286,7 +286,7 @@
     <t>227401/PR312929</t>
   </si>
   <si>
-    <t>C:/Users/paul.jones/Documents/GitHub/ModiffyEfficiency/ModiffyEfficiency/surveys\INIS-FSS-052820-006 (HRT 11-13).xlsx</t>
+    <t>C:\Users\paul.jones\Documents\GitHub\ModiffyEfficiency\ModiffyEfficiency\Output\Output Files\INIS-FSS-052820-006 (HRT 11-13).xlsx</t>
   </si>
   <si>
     <t>&lt;Worksheet "Systematic SDS"&gt;</t>
@@ -905,7 +905,7 @@
         <v>44183</v>
       </c>
       <c r="E14">
-        <v>0.3375</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -982,7 +982,7 @@
         <v>44219</v>
       </c>
       <c r="E18">
-        <v>0.53</v>
+        <v>0.13</v>
       </c>
       <c r="F18">
         <v>0.53</v>
@@ -1002,7 +1002,7 @@
         <v>44219</v>
       </c>
       <c r="E19">
-        <v>0.53</v>
+        <v>0.13</v>
       </c>
       <c r="F19">
         <v>0.53</v>
@@ -1022,7 +1022,7 @@
         <v>44219</v>
       </c>
       <c r="E20">
-        <v>0.53</v>
+        <v>0.13</v>
       </c>
       <c r="F20">
         <v>0.53</v>
@@ -1042,7 +1042,7 @@
         <v>44219</v>
       </c>
       <c r="E21">
-        <v>0.53</v>
+        <v>0.13</v>
       </c>
       <c r="F21">
         <v>0.53</v>
@@ -1062,7 +1062,7 @@
         <v>44219</v>
       </c>
       <c r="E22">
-        <v>0.53</v>
+        <v>0.13</v>
       </c>
       <c r="F22">
         <v>0.53</v>
@@ -1593,10 +1593,10 @@
         <v>44153</v>
       </c>
       <c r="E49">
-        <v>0.8</v>
+        <v>0.01</v>
       </c>
       <c r="F49">
-        <v>0.8</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -1613,10 +1613,10 @@
         <v>44153</v>
       </c>
       <c r="E50">
-        <v>0.8</v>
+        <v>0.01</v>
       </c>
       <c r="F50">
-        <v>0.8</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -1910,10 +1910,10 @@
         <v>44153</v>
       </c>
       <c r="E65">
-        <v>0.8</v>
+        <v>0.01</v>
       </c>
       <c r="F65">
-        <v>0.8</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="66" spans="1:6">

</xml_diff>